<commit_message>
compute shader sample v0.4.2 (GPU bandwidth) and v0.5.3 (GPU latency)
</commit_message>
<xml_diff>
--- a/simple_test_compute_shader/LowLevelBenchmarkingRTX3060Ti.xlsx
+++ b/simple_test_compute_shader/LowLevelBenchmarkingRTX3060Ti.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="54">
   <si>
     <t>Operation</t>
   </si>
@@ -378,13 +378,43 @@
   </si>
   <si>
     <t>Topology 512*512*16 give 40 ns. 512*512*32 give 289 ns, (unknown cache level?).  512*512*64 cause error, HRESULT=887A0005h</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Function  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Latency=F(size)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  is not monotone. This caused by shader compiler optimizations? Required GPU assembly shader?</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -428,6 +458,16 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -518,7 +558,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -547,14 +587,15 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -850,10 +891,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T35"/>
+  <dimension ref="A1:T36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29:T29"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1125,64 +1166,64 @@
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
     </row>
     <row r="18" spans="1:20">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
     </row>
     <row r="19" spans="1:20">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
     </row>
     <row r="20" spans="1:20">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
     </row>
     <row r="21" spans="1:20">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
     </row>
     <row r="22" spans="1:20">
       <c r="A22" s="11" t="s">
@@ -1243,6 +1284,20 @@
       <c r="D27" s="11"/>
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="12"/>
+      <c r="R27" s="12"/>
+      <c r="S27" s="12"/>
+      <c r="T27" s="12"/>
     </row>
     <row r="28" spans="1:20">
       <c r="A28" s="11" t="s">
@@ -1253,20 +1308,18 @@
       <c r="D28" s="11"/>
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
-      <c r="G28" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="15"/>
-      <c r="O28" s="15"/>
-      <c r="P28" s="15"/>
-      <c r="Q28" s="15"/>
-      <c r="R28" s="15"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
+      <c r="R28" s="10"/>
     </row>
     <row r="29" spans="1:20">
       <c r="A29" s="11" t="s">
@@ -1277,22 +1330,22 @@
       <c r="D29" s="11"/>
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
-      <c r="G29" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="15"/>
-      <c r="N29" s="15"/>
-      <c r="O29" s="15"/>
-      <c r="P29" s="15"/>
-      <c r="Q29" s="15"/>
-      <c r="R29" s="15"/>
-      <c r="S29" s="10"/>
-      <c r="T29" s="10"/>
+      <c r="G29" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10"/>
+      <c r="R29" s="10"/>
+      <c r="S29" s="12"/>
+      <c r="T29" s="12"/>
     </row>
     <row r="30" spans="1:20">
       <c r="A30" s="11" t="s">
@@ -1303,33 +1356,65 @@
       <c r="D30" s="11"/>
       <c r="E30" s="11"/>
       <c r="F30" s="11"/>
+      <c r="G30" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="10"/>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="10"/>
+      <c r="R30" s="10"/>
+      <c r="S30" s="12"/>
+      <c r="T30" s="12"/>
+    </row>
+    <row r="31" spans="1:20">
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="12"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="12"/>
+      <c r="P31" s="12"/>
+      <c r="Q31" s="12"/>
+      <c r="R31" s="12"/>
+      <c r="S31" s="12"/>
+      <c r="T31" s="12"/>
     </row>
     <row r="32" spans="1:20">
-      <c r="A32" s="10" t="s">
+      <c r="A32" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="10" t="s">
+      <c r="A33" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="10"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
+      <c r="A34" s="12"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="11" t="s">
@@ -1341,8 +1426,27 @@
       <c r="E35" s="11"/>
       <c r="F35" s="11"/>
     </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+    </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="25">
+    <mergeCell ref="G30:T30"/>
+    <mergeCell ref="G31:T31"/>
+    <mergeCell ref="G27:T27"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A24:F24"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="A28:F28"/>
+    <mergeCell ref="A22:F22"/>
     <mergeCell ref="G28:R28"/>
     <mergeCell ref="A35:F35"/>
     <mergeCell ref="G29:T29"/>
@@ -1359,11 +1463,6 @@
     <mergeCell ref="A21:F21"/>
     <mergeCell ref="A29:F29"/>
     <mergeCell ref="A23:F23"/>
-    <mergeCell ref="A24:F24"/>
-    <mergeCell ref="A25:F25"/>
-    <mergeCell ref="A27:F27"/>
-    <mergeCell ref="A28:F28"/>
-    <mergeCell ref="A22:F22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A15" r:id="rId1"/>

</xml_diff>

<commit_message>
compute shader sample v0.4.2 (GPU bandwidth) and v0.5.5 (GPU latency)
</commit_message>
<xml_diff>
--- a/simple_test_compute_shader/LowLevelBenchmarkingRTX3060Ti.xlsx
+++ b/simple_test_compute_shader/LowLevelBenchmarkingRTX3060Ti.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="v0.4.1 &amp; v0.5.1" sheetId="1" r:id="rId1"/>
+    <sheet name="v0.4.1 &amp; v0.5.5" sheetId="1" r:id="rId1"/>
     <sheet name="Лист1" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
   <si>
     <t>Operation</t>
   </si>
@@ -81,70 +81,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>(448 GBPS)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">*11 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(under construction)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">*10 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(under construction)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">*9 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(under construction)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">*12 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(under construction)</t>
     </r>
   </si>
   <si>
@@ -408,6 +344,24 @@
       </rPr>
       <t xml:space="preserve">  is not monotone. This caused by shader compiler optimizations? Required GPU assembly shader?</t>
     </r>
+  </si>
+  <si>
+    <t>Latency is very sensitive to random pattern.</t>
+  </si>
+  <si>
+    <t>Physical latency results updated at v0.5.5. Address increment mode experimentally selected as optimal.</t>
+  </si>
+  <si>
+    <t>*9 (under construction)</t>
+  </si>
+  <si>
+    <t>*10 (under construction)</t>
+  </si>
+  <si>
+    <t>*11 (under construction)</t>
+  </si>
+  <si>
+    <t>*12 (under construction)</t>
   </si>
 </sst>
 </file>
@@ -490,7 +444,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -550,6 +504,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -558,7 +521,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -578,15 +541,11 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -596,6 +555,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -891,11 +853,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T36"/>
+  <dimension ref="A1:T37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -905,7 +865,7 @@
     <col min="5" max="6" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30.75" customHeight="1">
+    <row r="1" spans="1:19" ht="30.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -925,9 +885,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:19">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>9</v>
@@ -945,9 +905,9 @@
         <v>21.65</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:19">
       <c r="A3" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>9</v>
@@ -956,7 +916,7 @@
         <v>24.12</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E3" s="6">
         <v>12.23</v>
@@ -965,9 +925,9 @@
         <v>20.96</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:19">
       <c r="A4" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>9</v>
@@ -976,7 +936,7 @@
         <v>426.83</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E4" s="6">
         <v>30.4</v>
@@ -985,9 +945,9 @@
         <v>20.48</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:19">
       <c r="A5" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>9</v>
@@ -996,7 +956,7 @@
         <v>19.25</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E5" s="6">
         <v>12.55</v>
@@ -1005,7 +965,7 @@
         <v>21.08</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:19">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
@@ -1016,7 +976,7 @@
         <v>209.35</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E6" s="6">
         <v>14.92</v>
@@ -1025,7 +985,7 @@
         <v>9.59</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:19">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
@@ -1036,7 +996,7 @@
         <v>19.309999999999999</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E7" s="6">
         <v>12.45</v>
@@ -1045,7 +1005,7 @@
         <v>9.74</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:19">
       <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
@@ -1056,7 +1016,7 @@
         <v>23.81</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E8" s="6">
         <v>12.44</v>
@@ -1065,7 +1025,7 @@
         <v>9.67</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:19">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -1076,7 +1036,7 @@
         <v>12.58</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E9" s="6">
         <v>9.41</v>
@@ -1085,67 +1045,82 @@
         <v>9.64</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:19">
+      <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="17">
         <v>1.89</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="8" t="s">
+      <c r="D10" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:19">
+      <c r="A11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="7">
         <v>24.39</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="8" t="s">
+      <c r="D11" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:19">
+      <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="6">
-        <v>40.85</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="8" t="s">
+      <c r="C12" s="17">
+        <v>71.19</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="6">
-        <v>40.270000000000003</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="F12" s="17">
+        <v>118.59</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="8"/>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13" s="4" t="s">
         <v>7</v>
       </c>
@@ -1153,21 +1128,36 @@
         <v>10</v>
       </c>
       <c r="C13" s="7">
-        <v>110.24</v>
+        <v>139.57</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>15</v>
       </c>
       <c r="F13" s="7">
-        <v>40.020000000000003</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>116.24</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
+    </row>
+    <row r="15" spans="1:19">
       <c r="A15" s="14" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
@@ -1175,9 +1165,9 @@
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:19">
       <c r="A16" s="13" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B16" s="12"/>
       <c r="C16" s="12"/>
@@ -1187,7 +1177,7 @@
     </row>
     <row r="18" spans="1:20">
       <c r="A18" s="15" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
@@ -1197,7 +1187,7 @@
     </row>
     <row r="19" spans="1:20">
       <c r="A19" s="12" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
@@ -1207,7 +1197,7 @@
     </row>
     <row r="20" spans="1:20">
       <c r="A20" s="12" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
@@ -1217,7 +1207,7 @@
     </row>
     <row r="21" spans="1:20">
       <c r="A21" s="12" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
@@ -1227,7 +1217,7 @@
     </row>
     <row r="22" spans="1:20">
       <c r="A22" s="11" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
@@ -1237,7 +1227,7 @@
     </row>
     <row r="23" spans="1:20">
       <c r="A23" s="11" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
@@ -1247,7 +1237,7 @@
     </row>
     <row r="24" spans="1:20">
       <c r="A24" s="11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
@@ -1257,7 +1247,7 @@
     </row>
     <row r="25" spans="1:20">
       <c r="A25" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -1267,7 +1257,7 @@
     </row>
     <row r="26" spans="1:20">
       <c r="A26" s="11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
@@ -1277,7 +1267,7 @@
     </row>
     <row r="27" spans="1:20">
       <c r="A27" s="11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
@@ -1301,7 +1291,7 @@
     </row>
     <row r="28" spans="1:20">
       <c r="A28" s="11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
@@ -1323,7 +1313,7 @@
     </row>
     <row r="29" spans="1:20">
       <c r="A29" s="11" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
@@ -1331,7 +1321,7 @@
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
       <c r="G29" s="10" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H29" s="10"/>
       <c r="I29" s="10"/>
@@ -1349,7 +1339,7 @@
     </row>
     <row r="30" spans="1:20">
       <c r="A30" s="11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
@@ -1357,7 +1347,7 @@
       <c r="E30" s="11"/>
       <c r="F30" s="11"/>
       <c r="G30" s="10" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H30" s="10"/>
       <c r="I30" s="10"/>
@@ -1391,7 +1381,7 @@
     </row>
     <row r="32" spans="1:20">
       <c r="A32" s="12" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
@@ -1401,7 +1391,7 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="12" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
@@ -1418,7 +1408,7 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="11" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
@@ -1428,7 +1418,7 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>
@@ -1436,33 +1426,45 @@
       <c r="E36" s="16"/>
       <c r="F36" s="16"/>
     </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+    </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="G30:T30"/>
-    <mergeCell ref="G31:T31"/>
-    <mergeCell ref="G27:T27"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="A24:F24"/>
-    <mergeCell ref="A25:F25"/>
-    <mergeCell ref="A27:F27"/>
-    <mergeCell ref="A28:F28"/>
-    <mergeCell ref="A22:F22"/>
-    <mergeCell ref="G28:R28"/>
-    <mergeCell ref="A35:F35"/>
-    <mergeCell ref="G29:T29"/>
-    <mergeCell ref="A16:F16"/>
+  <mergeCells count="28">
+    <mergeCell ref="A37:E37"/>
     <mergeCell ref="A15:F15"/>
     <mergeCell ref="A30:F30"/>
     <mergeCell ref="A32:F32"/>
     <mergeCell ref="A33:F33"/>
     <mergeCell ref="A18:F18"/>
-    <mergeCell ref="A34:E34"/>
     <mergeCell ref="A26:F26"/>
     <mergeCell ref="A19:F19"/>
     <mergeCell ref="A20:F20"/>
     <mergeCell ref="A21:F21"/>
     <mergeCell ref="A29:F29"/>
     <mergeCell ref="A23:F23"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="G12:R12"/>
+    <mergeCell ref="G13:S13"/>
+    <mergeCell ref="G28:R28"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="G29:T29"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="G30:T30"/>
+    <mergeCell ref="G31:T31"/>
+    <mergeCell ref="G27:T27"/>
+    <mergeCell ref="A24:F24"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="A28:F28"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A15" r:id="rId1"/>

</xml_diff>

<commit_message>
compute shader sample v0.6.1 (GPU latency with shader monitoring)
</commit_message>
<xml_diff>
--- a/simple_test_compute_shader/LowLevelBenchmarkingRTX3060Ti.xlsx
+++ b/simple_test_compute_shader/LowLevelBenchmarkingRTX3060Ti.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
   <si>
     <t>Operation</t>
   </si>
@@ -363,12 +363,18 @@
   <si>
     <t>*12 (under construction)</t>
   </si>
+  <si>
+    <t>https://github.com/manusov/LearningVisualStudio/tree/master/simple_test_compute_shader/GPU_LATENCY_WITH_SHADER_MONITORING</t>
+  </si>
+  <si>
+    <t>Variant (v0.6.1+) with monitoring shader execution and speculative effects, include break cycle in the shader:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -428,6 +434,21 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="3">
@@ -521,7 +542,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -545,6 +566,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -552,12 +576,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -853,7 +878,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T37"/>
+  <dimension ref="A1:T39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1052,16 +1077,16 @@
       <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="9">
         <v>1.89</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="9" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1092,32 +1117,32 @@
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C12" s="9">
         <v>71.19</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="17">
+      <c r="F12" s="9">
         <v>118.59</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="10"/>
-      <c r="R12" s="10"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
       <c r="S12" s="8"/>
     </row>
     <row r="13" spans="1:19">
@@ -1139,339 +1164,362 @@
       <c r="F13" s="7">
         <v>116.24</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="10"/>
-      <c r="R13" s="10"/>
-      <c r="S13" s="10"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="11"/>
     </row>
     <row r="15" spans="1:19">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
     </row>
     <row r="16" spans="1:19">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+    </row>
+    <row r="17" spans="1:20">
+      <c r="A17" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
     </row>
     <row r="18" spans="1:20">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+    </row>
+    <row r="20" spans="1:20">
+      <c r="A20" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-    </row>
-    <row r="19" spans="1:20">
-      <c r="A19" s="12" t="s">
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="A21" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-    </row>
-    <row r="20" spans="1:20">
-      <c r="A20" s="12" t="s">
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+    </row>
+    <row r="22" spans="1:20">
+      <c r="A22" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-    </row>
-    <row r="21" spans="1:20">
-      <c r="A21" s="12" t="s">
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+    </row>
+    <row r="23" spans="1:20">
+      <c r="A23" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-    </row>
-    <row r="22" spans="1:20">
-      <c r="A22" s="11" t="s">
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+    </row>
+    <row r="24" spans="1:20">
+      <c r="A24" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-    </row>
-    <row r="23" spans="1:20">
-      <c r="A23" s="11" t="s">
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+    </row>
+    <row r="25" spans="1:20">
+      <c r="A25" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-    </row>
-    <row r="24" spans="1:20">
-      <c r="A24" s="11" t="s">
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+    </row>
+    <row r="26" spans="1:20">
+      <c r="A26" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-    </row>
-    <row r="25" spans="1:20">
-      <c r="A25" s="11" t="s">
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+    </row>
+    <row r="27" spans="1:20">
+      <c r="A27" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-    </row>
-    <row r="26" spans="1:20">
-      <c r="A26" s="11" t="s">
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+    </row>
+    <row r="28" spans="1:20">
+      <c r="A28" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-    </row>
-    <row r="27" spans="1:20">
-      <c r="A27" s="11" t="s">
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+    </row>
+    <row r="29" spans="1:20">
+      <c r="A29" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
-      <c r="L27" s="12"/>
-      <c r="M27" s="12"/>
-      <c r="N27" s="12"/>
-      <c r="O27" s="12"/>
-      <c r="P27" s="12"/>
-      <c r="Q27" s="12"/>
-      <c r="R27" s="12"/>
-      <c r="S27" s="12"/>
-      <c r="T27" s="12"/>
-    </row>
-    <row r="28" spans="1:20">
-      <c r="A28" s="11" t="s">
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="13"/>
+      <c r="P29" s="13"/>
+      <c r="Q29" s="13"/>
+      <c r="R29" s="13"/>
+      <c r="S29" s="13"/>
+      <c r="T29" s="13"/>
+    </row>
+    <row r="30" spans="1:20">
+      <c r="A30" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
-      <c r="K28" s="10"/>
-      <c r="L28" s="10"/>
-      <c r="M28" s="10"/>
-      <c r="N28" s="10"/>
-      <c r="O28" s="10"/>
-      <c r="P28" s="10"/>
-      <c r="Q28" s="10"/>
-      <c r="R28" s="10"/>
-    </row>
-    <row r="29" spans="1:20">
-      <c r="A29" s="11" t="s">
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="11"/>
+      <c r="R30" s="11"/>
+    </row>
+    <row r="31" spans="1:20">
+      <c r="A31" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="10" t="s">
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10"/>
-      <c r="M29" s="10"/>
-      <c r="N29" s="10"/>
-      <c r="O29" s="10"/>
-      <c r="P29" s="10"/>
-      <c r="Q29" s="10"/>
-      <c r="R29" s="10"/>
-      <c r="S29" s="12"/>
-      <c r="T29" s="12"/>
-    </row>
-    <row r="30" spans="1:20">
-      <c r="A30" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10"/>
-      <c r="N30" s="10"/>
-      <c r="O30" s="10"/>
-      <c r="P30" s="10"/>
-      <c r="Q30" s="10"/>
-      <c r="R30" s="10"/>
-      <c r="S30" s="12"/>
-      <c r="T30" s="12"/>
-    </row>
-    <row r="31" spans="1:20">
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="12"/>
-      <c r="K31" s="12"/>
-      <c r="L31" s="12"/>
-      <c r="M31" s="12"/>
-      <c r="N31" s="12"/>
-      <c r="O31" s="12"/>
-      <c r="P31" s="12"/>
-      <c r="Q31" s="12"/>
-      <c r="R31" s="12"/>
-      <c r="S31" s="12"/>
-      <c r="T31" s="12"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="11"/>
+      <c r="Q31" s="11"/>
+      <c r="R31" s="11"/>
+      <c r="S31" s="13"/>
+      <c r="T31" s="13"/>
     </row>
     <row r="32" spans="1:20">
       <c r="A32" s="12" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
       <c r="D32" s="12"/>
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="12" t="s">
+      <c r="G32" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="11"/>
+      <c r="P32" s="11"/>
+      <c r="Q32" s="11"/>
+      <c r="R32" s="11"/>
+      <c r="S32" s="13"/>
+      <c r="T32" s="13"/>
+    </row>
+    <row r="33" spans="1:20">
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="13"/>
+      <c r="O33" s="13"/>
+      <c r="P33" s="13"/>
+      <c r="Q33" s="13"/>
+      <c r="R33" s="13"/>
+      <c r="S33" s="13"/>
+      <c r="T33" s="13"/>
+    </row>
+    <row r="34" spans="1:20">
+      <c r="A34" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+    </row>
+    <row r="35" spans="1:20">
+      <c r="A35" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="11" t="s">
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+    </row>
+    <row r="36" spans="1:20">
+      <c r="A36" s="13"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+    </row>
+    <row r="37" spans="1:20">
+      <c r="A37" s="12" t="s">
         <v>47</v>
-      </c>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="B36" s="16"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="10" t="s">
-        <v>50</v>
       </c>
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
       <c r="D37" s="12"/>
       <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+    </row>
+    <row r="38" spans="1:20">
+      <c r="A38" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+    </row>
+    <row r="39" spans="1:20">
+      <c r="A39" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="A37:E37"/>
+  <mergeCells count="30">
+    <mergeCell ref="A39:E39"/>
     <mergeCell ref="A15:F15"/>
-    <mergeCell ref="A30:F30"/>
     <mergeCell ref="A32:F32"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="A26:F26"/>
-    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A35:F35"/>
     <mergeCell ref="A20:F20"/>
+    <mergeCell ref="A28:F28"/>
     <mergeCell ref="A21:F21"/>
-    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A22:F22"/>
     <mergeCell ref="A23:F23"/>
-    <mergeCell ref="A22:F22"/>
-    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="A24:F24"/>
+    <mergeCell ref="A38:F38"/>
     <mergeCell ref="G12:R12"/>
     <mergeCell ref="G13:S13"/>
-    <mergeCell ref="G28:R28"/>
-    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="G30:R30"/>
+    <mergeCell ref="A37:F37"/>
+    <mergeCell ref="G31:T31"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A36:E36"/>
+    <mergeCell ref="G32:T32"/>
+    <mergeCell ref="G33:T33"/>
     <mergeCell ref="G29:T29"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A34:E34"/>
-    <mergeCell ref="G30:T30"/>
-    <mergeCell ref="G31:T31"/>
-    <mergeCell ref="G27:T27"/>
-    <mergeCell ref="A24:F24"/>
-    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="A26:F26"/>
     <mergeCell ref="A27:F27"/>
-    <mergeCell ref="A28:F28"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A30:F30"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="A18:F18"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A15" r:id="rId1"/>
     <hyperlink ref="A16" r:id="rId2"/>
+    <hyperlink ref="A18" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>